<commit_message>
Add last number date to new cycle
</commit_message>
<xml_diff>
--- a/Documents/CycleAnalisys.xlsx
+++ b/Documents/CycleAnalisys.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\mega-sena\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A4ADE8-6871-46B6-BB15-B89BAB56CDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA6CA83-2179-4DD9-A2B5-468AADFD4744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F929A58B-8040-4F54-9AC6-2C5D8415EDC6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F929A58B-8040-4F54-9AC6-2C5D8415EDC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,26 +35,9 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,56 +53,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -135,43 +74,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -192,16 +103,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -213,22 +114,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A562C091-76F2-4E41-9C45-27AC10434A39}" name="Table1" displayName="Table1" ref="A1:D1048576" totalsRowShown="0">
-  <autoFilter ref="A1:D1048576" xr:uid="{A562C091-76F2-4E41-9C45-27AC10434A39}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D65">
-    <sortCondition ref="D1:D1048576"/>
-  </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4A549C37-1684-4AB4-95AB-FB963C5C3DD9}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{AEDE7474-4205-4D2E-8D6E-2FB2FA520801}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{C11BA03B-D611-4B87-9670-8391E485B863}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{9AB22124-CA7F-4ADD-BBE0-E726476186A0}" name="Column4"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,7 +415,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B50063-9344-4572-8551-DC0076C3C064}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3220,896 +3107,14 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:L61">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="B2:N61">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M2:N61">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EEEE5F5-6FD8-453A-949D-046D1B967CB3}">
-  <dimension ref="A1:D61"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>12</v>
-      </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>21</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>19</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>40</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>52</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>20</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>24</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>25</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>33</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>46</v>
-      </c>
-      <c r="B18" s="8">
-        <v>2</v>
-      </c>
-      <c r="C18" s="8">
-        <v>2</v>
-      </c>
-      <c r="D18" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>47</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>51</v>
-      </c>
-      <c r="B20" s="4">
-        <v>2</v>
-      </c>
-      <c r="C20" s="4">
-        <v>3</v>
-      </c>
-      <c r="D20" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>54</v>
-      </c>
-      <c r="B21">
-        <v>3</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
-        <v>55</v>
-      </c>
-      <c r="B22" s="8">
-        <v>2</v>
-      </c>
-      <c r="C22" s="8">
-        <v>2</v>
-      </c>
-      <c r="D22" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>57</v>
-      </c>
-      <c r="B23">
-        <v>3</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>2</v>
-      </c>
-      <c r="B24">
-        <v>4</v>
-      </c>
-      <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
-        <v>11</v>
-      </c>
-      <c r="B25" s="8">
-        <v>3</v>
-      </c>
-      <c r="C25" s="8">
-        <v>3</v>
-      </c>
-      <c r="D25" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>16</v>
-      </c>
-      <c r="B26">
-        <v>4</v>
-      </c>
-      <c r="C26">
-        <v>4</v>
-      </c>
-      <c r="D26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>4</v>
-      </c>
-      <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="D27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>29</v>
-      </c>
-      <c r="B28">
-        <v>4</v>
-      </c>
-      <c r="C28">
-        <v>4</v>
-      </c>
-      <c r="D28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>30</v>
-      </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
-        <v>34</v>
-      </c>
-      <c r="B30">
-        <v>4</v>
-      </c>
-      <c r="C30">
-        <v>4</v>
-      </c>
-      <c r="D30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>37</v>
-      </c>
-      <c r="B31">
-        <v>4</v>
-      </c>
-      <c r="C31">
-        <v>4</v>
-      </c>
-      <c r="D31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>38</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="C32">
-        <v>4</v>
-      </c>
-      <c r="D32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>42</v>
-      </c>
-      <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="C33">
-        <v>4</v>
-      </c>
-      <c r="D33">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>43</v>
-      </c>
-      <c r="B34">
-        <v>4</v>
-      </c>
-      <c r="C34">
-        <v>4</v>
-      </c>
-      <c r="D34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
-        <v>53</v>
-      </c>
-      <c r="B35" s="8">
-        <v>2</v>
-      </c>
-      <c r="C35" s="8">
-        <v>3</v>
-      </c>
-      <c r="D35" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
-        <v>60</v>
-      </c>
-      <c r="B36" s="10">
-        <v>2</v>
-      </c>
-      <c r="C36" s="10">
-        <v>3</v>
-      </c>
-      <c r="D36" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>6</v>
-      </c>
-      <c r="B37">
-        <v>5</v>
-      </c>
-      <c r="C37">
-        <v>5</v>
-      </c>
-      <c r="D37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>27</v>
-      </c>
-      <c r="B38">
-        <v>4</v>
-      </c>
-      <c r="C38">
-        <v>5</v>
-      </c>
-      <c r="D38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>28</v>
-      </c>
-      <c r="B39">
-        <v>5</v>
-      </c>
-      <c r="C39">
-        <v>5</v>
-      </c>
-      <c r="D39">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>41</v>
-      </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
-      <c r="C40">
-        <v>5</v>
-      </c>
-      <c r="D40">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>44</v>
-      </c>
-      <c r="B41">
-        <v>5</v>
-      </c>
-      <c r="C41">
-        <v>5</v>
-      </c>
-      <c r="D41">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>45</v>
-      </c>
-      <c r="B42">
-        <v>5</v>
-      </c>
-      <c r="C42">
-        <v>5</v>
-      </c>
-      <c r="D42">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>49</v>
-      </c>
-      <c r="B43">
-        <v>5</v>
-      </c>
-      <c r="C43">
-        <v>5</v>
-      </c>
-      <c r="D43">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>50</v>
-      </c>
-      <c r="B44">
-        <v>5</v>
-      </c>
-      <c r="C44">
-        <v>5</v>
-      </c>
-      <c r="D44">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
-        <v>56</v>
-      </c>
-      <c r="B45">
-        <v>5</v>
-      </c>
-      <c r="C45">
-        <v>5</v>
-      </c>
-      <c r="D45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>8</v>
-      </c>
-      <c r="B46">
-        <v>6</v>
-      </c>
-      <c r="C46">
-        <v>6</v>
-      </c>
-      <c r="D46">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>22</v>
-      </c>
-      <c r="B47">
-        <v>6</v>
-      </c>
-      <c r="C47">
-        <v>6</v>
-      </c>
-      <c r="D47">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>31</v>
-      </c>
-      <c r="B48">
-        <v>6</v>
-      </c>
-      <c r="C48">
-        <v>6</v>
-      </c>
-      <c r="D48">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>35</v>
-      </c>
-      <c r="B49">
-        <v>6</v>
-      </c>
-      <c r="C49">
-        <v>6</v>
-      </c>
-      <c r="D49">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
-        <v>39</v>
-      </c>
-      <c r="B50" s="4">
-        <v>5</v>
-      </c>
-      <c r="C50" s="4">
-        <v>6</v>
-      </c>
-      <c r="D50" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>48</v>
-      </c>
-      <c r="B51">
-        <v>6</v>
-      </c>
-      <c r="C51">
-        <v>6</v>
-      </c>
-      <c r="D51">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
-        <v>5</v>
-      </c>
-      <c r="B52" s="4">
-        <v>6</v>
-      </c>
-      <c r="C52" s="4">
-        <v>7</v>
-      </c>
-      <c r="D52" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>9</v>
-      </c>
-      <c r="B53">
-        <v>7</v>
-      </c>
-      <c r="C53">
-        <v>7</v>
-      </c>
-      <c r="D53">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>10</v>
-      </c>
-      <c r="B54">
-        <v>7</v>
-      </c>
-      <c r="C54">
-        <v>7</v>
-      </c>
-      <c r="D54">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
-        <v>13</v>
-      </c>
-      <c r="B55" s="4">
-        <v>6</v>
-      </c>
-      <c r="C55" s="4">
-        <v>7</v>
-      </c>
-      <c r="D55" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>14</v>
-      </c>
-      <c r="B56">
-        <v>7</v>
-      </c>
-      <c r="C56">
-        <v>7</v>
-      </c>
-      <c r="D56">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>23</v>
-      </c>
-      <c r="B57">
-        <v>7</v>
-      </c>
-      <c r="C57">
-        <v>7</v>
-      </c>
-      <c r="D57">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>32</v>
-      </c>
-      <c r="B58">
-        <v>6</v>
-      </c>
-      <c r="C58">
-        <v>7</v>
-      </c>
-      <c r="D58">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="7">
-        <v>36</v>
-      </c>
-      <c r="B59" s="8">
-        <v>5</v>
-      </c>
-      <c r="C59" s="8">
-        <v>6</v>
-      </c>
-      <c r="D59" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="3">
-        <v>58</v>
-      </c>
-      <c r="B60" s="4">
-        <v>6</v>
-      </c>
-      <c r="C60" s="4">
-        <v>7</v>
-      </c>
-      <c r="D60" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>59</v>
-      </c>
-      <c r="B61">
-        <v>9</v>
-      </c>
-      <c r="C61">
-        <v>9</v>
-      </c>
-      <c r="D61">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add cycle time numbers medium
</commit_message>
<xml_diff>
--- a/Documents/CycleAnalisys.xlsx
+++ b/Documents/CycleAnalisys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\mega-sena\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46828265-BA8E-463B-94E2-AB5C6A48E968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F95CB58B-3FB3-412A-8F77-B05BCC0C14E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F929A58B-8040-4F54-9AC6-2C5D8415EDC6}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3165,21 +3166,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41812CA6-D374-44FF-99BD-D31D26E35E53}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -3189,8 +3193,26 @@
       <c r="C2" s="3">
         <v>45274</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="9">
+        <v>21</v>
+      </c>
+      <c r="F2" s="4">
+        <v>24</v>
+      </c>
+      <c r="G2" s="4">
+        <v>33</v>
+      </c>
+      <c r="H2" s="9">
+        <v>41</v>
+      </c>
+      <c r="I2" s="4">
+        <v>48</v>
+      </c>
+      <c r="J2" s="9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3201,7 +3223,7 @@
         <v>45209</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -3212,7 +3234,7 @@
         <v>45267</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -3223,7 +3245,7 @@
         <v>45276</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -3234,7 +3256,7 @@
         <v>45269</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -3245,7 +3267,7 @@
         <v>45258</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -3256,7 +3278,7 @@
         <v>45276</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -3267,7 +3289,7 @@
         <v>45272</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -3278,7 +3300,7 @@
         <v>45227</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3289,7 +3311,7 @@
         <v>45241</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -3300,7 +3322,7 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -3311,7 +3333,7 @@
         <v>45265</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -3322,7 +3344,7 @@
         <v>45255</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -3333,7 +3355,7 @@
         <v>45267</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -3404,10 +3426,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" s="3">
-        <v>45272</v>
+        <v>45291</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3433,14 +3455,14 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="B25" s="4">
-        <v>0</v>
+      <c r="B25" s="7">
+        <v>1</v>
       </c>
       <c r="C25" s="3">
-        <v>45244</v>
+        <v>45291</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3532,14 +3554,14 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
+      <c r="A34" s="6">
         <v>33</v>
       </c>
-      <c r="B34" s="4">
-        <v>0</v>
+      <c r="B34" s="7">
+        <v>1</v>
       </c>
       <c r="C34" s="3">
-        <v>45248</v>
+        <v>45291</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3624,10 +3646,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C42" s="3">
-        <v>45274</v>
+        <v>45291</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -3697,14 +3719,14 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
+      <c r="A49" s="6">
         <v>48</v>
       </c>
-      <c r="B49" s="12">
-        <v>0</v>
+      <c r="B49" s="7">
+        <v>1</v>
       </c>
       <c r="C49" s="3">
-        <v>45237</v>
+        <v>45291</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3789,10 +3811,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C57" s="3">
-        <v>45274</v>
+        <v>45291</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>